<commit_message>
resolve import file bug and validate file header
</commit_message>
<xml_diff>
--- a/Onyx/wwwroot/formats/Emp_Attendance_Import_Sample.xlsx
+++ b/Onyx/wwwroot/formats/Emp_Attendance_Import_Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HRMS\Onyx\Onyx\wwwroot\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44208AB-E1D2-46C9-884C-1F1B72AF4F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16099B2-7D3D-45A6-9F99-56826B976A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="1896" windowWidth="17280" windowHeight="8880" xr2:uid="{E50CF398-DA2C-4B7D-84AE-DC8FC7B7A6A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E50CF398-DA2C-4B7D-84AE-DC8FC7B7A6A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>No Of Days</t>
   </si>
@@ -45,25 +45,16 @@
     <t>Unpaid</t>
   </si>
   <si>
-    <t>Payable</t>
-  </si>
-  <si>
-    <t>NHrs</t>
-  </si>
-  <si>
     <t>W.OT</t>
   </si>
   <si>
     <t>H.OT</t>
   </si>
   <si>
-    <t>Loan Recovery</t>
-  </si>
-  <si>
     <t>XXX</t>
   </si>
   <si>
-    <t>EmpCd</t>
+    <t>Employee Code</t>
   </si>
 </sst>
 </file>
@@ -427,12 +418,12 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.77734375" customWidth="1"/>
     <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
@@ -440,7 +431,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -457,19 +448,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -484,15 +467,6 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
         <v>0</v>
       </c>
     </row>

</xml_diff>